<commit_message>
New query for LAST_POKEMON_BY_TYPE
</commit_message>
<xml_diff>
--- a/Part_4_Progress.xlsx
+++ b/Part_4_Progress.xlsx
@@ -352,7 +352,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp7.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$A$13" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$A$13" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp8.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1314,7 +1314,7 @@
   <dimension ref="A1:C29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1403,7 +1403,9 @@
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="2"/>
+      <c r="A13" s="2" t="b">
+        <v>1</v>
+      </c>
       <c r="B13" t="s">
         <v>23</v>
       </c>

</xml_diff>

<commit_message>
New query for Union
May or may not keep this query...
</commit_message>
<xml_diff>
--- a/Part_4_Progress.xlsx
+++ b/Part_4_Progress.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>10 SQL Retrieval Queries</t>
   </si>
@@ -109,6 +109,9 @@
   </si>
   <si>
     <t>Average weight of pokemon</t>
+  </si>
+  <si>
+    <t>Heaviest and lightest Pokemon</t>
   </si>
 </sst>
 </file>
@@ -348,7 +351,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp6.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$A$11" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$A$11" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp7.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1314,7 +1317,7 @@
   <dimension ref="A1:C29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1394,7 +1397,12 @@
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="2"/>
+      <c r="A11" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="B11" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>

</xml_diff>

<commit_message>
Updated queries, add new one
Changed database type of Height and Weight to Int and Float respectively
to simplify queries.
New query for Earthquake
</commit_message>
<xml_diff>
--- a/Part_4_Progress.xlsx
+++ b/Part_4_Progress.xlsx
@@ -347,7 +347,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp5.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$A$9" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$A$9" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp6.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1385,7 +1385,9 @@
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="2"/>
+      <c r="A9" s="2" t="b">
+        <v>1</v>
+      </c>
       <c r="B9" t="s">
         <v>22</v>
       </c>

</xml_diff>

<commit_message>
Added Queries and Log
Added Insert and Delete Queries and Log of all queries (Except for
switching descriptions) for small database (Synthetic data).
</commit_message>
<xml_diff>
--- a/Part_4_Progress.xlsx
+++ b/Part_4_Progress.xlsx
@@ -1,22 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="150" windowWidth="20115" windowHeight="7995"/>
+    <workbookView xWindow="240" yWindow="160" windowWidth="16400" windowHeight="17240"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t>10 SQL Retrieval Queries</t>
   </si>
@@ -57,15 +62,9 @@
     <t>Two Inserts</t>
   </si>
   <si>
-    <t>insert 2 pokemon from Generation 3</t>
-  </si>
-  <si>
     <t>switch Generation 5 description to Generation 1 description</t>
   </si>
   <si>
-    <t>(possibly) delete the 2 new insertions from Gen 3</t>
-  </si>
-  <si>
     <t>one "Aggregate" query</t>
   </si>
   <si>
@@ -112,6 +111,18 @@
   </si>
   <si>
     <t>Heaviest and lightest Pokemon</t>
+  </si>
+  <si>
+    <t>Insert Treecko</t>
+  </si>
+  <si>
+    <t>Insert Mudkip</t>
+  </si>
+  <si>
+    <t>Delete Treecko</t>
+  </si>
+  <si>
+    <t>Delete Mudkip</t>
   </si>
 </sst>
 </file>
@@ -320,19 +331,19 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp13.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$A$25" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$A$25" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp14.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$A$26" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$A$26" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp15.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$A$28" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$A$28" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp16.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$A$29" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$A$29" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -376,13 +387,13 @@
           <xdr:col>0</xdr:col>
           <xdr:colOff>419100</xdr:colOff>
           <xdr:row>2</xdr:row>
-          <xdr:rowOff>171450</xdr:rowOff>
+          <xdr:rowOff>177800</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>0</xdr:col>
           <xdr:colOff>723900</xdr:colOff>
           <xdr:row>4</xdr:row>
-          <xdr:rowOff>9525</xdr:rowOff>
+          <xdr:rowOff>12700</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -417,13 +428,13 @@
           <xdr:col>0</xdr:col>
           <xdr:colOff>419100</xdr:colOff>
           <xdr:row>3</xdr:row>
-          <xdr:rowOff>171450</xdr:rowOff>
+          <xdr:rowOff>177800</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>0</xdr:col>
           <xdr:colOff>723900</xdr:colOff>
           <xdr:row>5</xdr:row>
-          <xdr:rowOff>9525</xdr:rowOff>
+          <xdr:rowOff>12700</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -458,13 +469,13 @@
           <xdr:col>0</xdr:col>
           <xdr:colOff>419100</xdr:colOff>
           <xdr:row>4</xdr:row>
-          <xdr:rowOff>171450</xdr:rowOff>
+          <xdr:rowOff>177800</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>0</xdr:col>
           <xdr:colOff>723900</xdr:colOff>
           <xdr:row>6</xdr:row>
-          <xdr:rowOff>9525</xdr:rowOff>
+          <xdr:rowOff>12700</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -499,13 +510,13 @@
           <xdr:col>0</xdr:col>
           <xdr:colOff>419100</xdr:colOff>
           <xdr:row>6</xdr:row>
-          <xdr:rowOff>171450</xdr:rowOff>
+          <xdr:rowOff>177800</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>0</xdr:col>
           <xdr:colOff>723900</xdr:colOff>
           <xdr:row>8</xdr:row>
-          <xdr:rowOff>9525</xdr:rowOff>
+          <xdr:rowOff>12700</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -540,13 +551,13 @@
           <xdr:col>0</xdr:col>
           <xdr:colOff>419100</xdr:colOff>
           <xdr:row>7</xdr:row>
-          <xdr:rowOff>171450</xdr:rowOff>
+          <xdr:rowOff>177800</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>0</xdr:col>
           <xdr:colOff>723900</xdr:colOff>
           <xdr:row>9</xdr:row>
-          <xdr:rowOff>9525</xdr:rowOff>
+          <xdr:rowOff>12700</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -581,13 +592,13 @@
           <xdr:col>0</xdr:col>
           <xdr:colOff>419100</xdr:colOff>
           <xdr:row>9</xdr:row>
-          <xdr:rowOff>171450</xdr:rowOff>
+          <xdr:rowOff>177800</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>0</xdr:col>
           <xdr:colOff>723900</xdr:colOff>
           <xdr:row>11</xdr:row>
-          <xdr:rowOff>9525</xdr:rowOff>
+          <xdr:rowOff>12700</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -622,13 +633,13 @@
           <xdr:col>0</xdr:col>
           <xdr:colOff>419100</xdr:colOff>
           <xdr:row>11</xdr:row>
-          <xdr:rowOff>171450</xdr:rowOff>
+          <xdr:rowOff>177800</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>0</xdr:col>
           <xdr:colOff>723900</xdr:colOff>
           <xdr:row>13</xdr:row>
-          <xdr:rowOff>9525</xdr:rowOff>
+          <xdr:rowOff>12700</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -663,13 +674,13 @@
           <xdr:col>0</xdr:col>
           <xdr:colOff>419100</xdr:colOff>
           <xdr:row>13</xdr:row>
-          <xdr:rowOff>171450</xdr:rowOff>
+          <xdr:rowOff>177800</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>0</xdr:col>
           <xdr:colOff>723900</xdr:colOff>
           <xdr:row>15</xdr:row>
-          <xdr:rowOff>9525</xdr:rowOff>
+          <xdr:rowOff>12700</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -704,13 +715,13 @@
           <xdr:col>0</xdr:col>
           <xdr:colOff>419100</xdr:colOff>
           <xdr:row>15</xdr:row>
-          <xdr:rowOff>171450</xdr:rowOff>
+          <xdr:rowOff>177800</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>0</xdr:col>
           <xdr:colOff>723900</xdr:colOff>
           <xdr:row>17</xdr:row>
-          <xdr:rowOff>9525</xdr:rowOff>
+          <xdr:rowOff>12700</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -745,13 +756,13 @@
           <xdr:col>0</xdr:col>
           <xdr:colOff>419100</xdr:colOff>
           <xdr:row>17</xdr:row>
-          <xdr:rowOff>171450</xdr:rowOff>
+          <xdr:rowOff>177800</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>0</xdr:col>
           <xdr:colOff>723900</xdr:colOff>
           <xdr:row>19</xdr:row>
-          <xdr:rowOff>9525</xdr:rowOff>
+          <xdr:rowOff>12700</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -786,13 +797,13 @@
           <xdr:col>0</xdr:col>
           <xdr:colOff>419100</xdr:colOff>
           <xdr:row>20</xdr:row>
-          <xdr:rowOff>171450</xdr:rowOff>
+          <xdr:rowOff>177800</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>0</xdr:col>
           <xdr:colOff>723900</xdr:colOff>
           <xdr:row>22</xdr:row>
-          <xdr:rowOff>9525</xdr:rowOff>
+          <xdr:rowOff>12700</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -827,13 +838,13 @@
           <xdr:col>0</xdr:col>
           <xdr:colOff>419100</xdr:colOff>
           <xdr:row>21</xdr:row>
-          <xdr:rowOff>171450</xdr:rowOff>
+          <xdr:rowOff>177800</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>0</xdr:col>
           <xdr:colOff>723900</xdr:colOff>
           <xdr:row>23</xdr:row>
-          <xdr:rowOff>9525</xdr:rowOff>
+          <xdr:rowOff>12700</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -868,13 +879,13 @@
           <xdr:col>0</xdr:col>
           <xdr:colOff>419100</xdr:colOff>
           <xdr:row>23</xdr:row>
-          <xdr:rowOff>171450</xdr:rowOff>
+          <xdr:rowOff>177800</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>0</xdr:col>
           <xdr:colOff>723900</xdr:colOff>
           <xdr:row>25</xdr:row>
-          <xdr:rowOff>9525</xdr:rowOff>
+          <xdr:rowOff>12700</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -909,13 +920,13 @@
           <xdr:col>0</xdr:col>
           <xdr:colOff>419100</xdr:colOff>
           <xdr:row>24</xdr:row>
-          <xdr:rowOff>171450</xdr:rowOff>
+          <xdr:rowOff>177800</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>0</xdr:col>
           <xdr:colOff>723900</xdr:colOff>
           <xdr:row>26</xdr:row>
-          <xdr:rowOff>9525</xdr:rowOff>
+          <xdr:rowOff>12700</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -950,13 +961,13 @@
           <xdr:col>0</xdr:col>
           <xdr:colOff>419100</xdr:colOff>
           <xdr:row>26</xdr:row>
-          <xdr:rowOff>171450</xdr:rowOff>
+          <xdr:rowOff>177800</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>0</xdr:col>
           <xdr:colOff>723900</xdr:colOff>
           <xdr:row>28</xdr:row>
-          <xdr:rowOff>9525</xdr:rowOff>
+          <xdr:rowOff>12700</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -991,13 +1002,13 @@
           <xdr:col>0</xdr:col>
           <xdr:colOff>419100</xdr:colOff>
           <xdr:row>27</xdr:row>
-          <xdr:rowOff>171450</xdr:rowOff>
+          <xdr:rowOff>177800</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>0</xdr:col>
           <xdr:colOff>723900</xdr:colOff>
           <xdr:row>29</xdr:row>
-          <xdr:rowOff>9525</xdr:rowOff>
+          <xdr:rowOff>12700</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1317,17 +1328,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="23" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="123.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="123.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -1338,184 +1349,198 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3">
       <c r="A3" s="3"/>
       <c r="B3" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3">
       <c r="A4" s="2" t="b">
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
       <c r="A5" s="2" t="b">
         <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
       <c r="A6" s="2" t="b">
         <v>1</v>
       </c>
       <c r="B6" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
       <c r="A7" s="2"/>
       <c r="B7" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
       <c r="A8" s="2" t="b">
         <v>1</v>
       </c>
       <c r="B8" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
       <c r="A9" s="2" t="b">
         <v>1</v>
       </c>
       <c r="B9" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
       <c r="A10" s="2"/>
       <c r="B10" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
       <c r="A11" s="2" t="b">
         <v>1</v>
       </c>
       <c r="B11" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
       <c r="A12" s="2"/>
       <c r="B12" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
       <c r="A13" s="2" t="b">
         <v>1</v>
       </c>
       <c r="B13" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
       <c r="A14" s="2"/>
       <c r="B14" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
       <c r="A15" s="2" t="b">
         <v>1</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
       <c r="A16" s="2"/>
       <c r="B16" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
       <c r="A17" s="2" t="b">
         <v>1</v>
       </c>
       <c r="B17" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
       <c r="A18" s="2"/>
       <c r="B18" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
       <c r="A19" s="2" t="b">
         <v>1</v>
       </c>
       <c r="B19" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
       <c r="A20" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2">
       <c r="A21" s="2"/>
       <c r="B21" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2">
       <c r="A22" s="2" t="b">
         <v>0</v>
       </c>
       <c r="B22" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
       <c r="A23" s="2"/>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2">
       <c r="A24" s="2"/>
       <c r="B24" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="2"/>
+    <row r="25" spans="1:2">
+      <c r="A25" s="2" t="b">
+        <v>1</v>
+      </c>
       <c r="B25" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" s="2"/>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2">
+      <c r="A26" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="B26" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2">
       <c r="A27" s="2"/>
       <c r="B27" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" s="2"/>
+    <row r="28" spans="1:2">
+      <c r="A28" s="2" t="b">
+        <v>1</v>
+      </c>
       <c r="B28" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" s="2"/>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2">
+      <c r="A29" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="B29" t="s">
+        <v>27</v>
+      </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B4:C4">
@@ -1599,367 +1624,389 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
-  <legacyDrawing r:id="rId3"/>
+  <pageSetup orientation="portrait"/>
+  <drawing r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x14">
       <controls>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1025" r:id="rId4" name="Check Box 1">
+            <control shapeId="1025" r:id="rId3" name="Check Box 1">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>0</xdr:col>
                     <xdr:colOff>419100</xdr:colOff>
                     <xdr:row>2</xdr:row>
-                    <xdr:rowOff>171450</xdr:rowOff>
+                    <xdr:rowOff>177800</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>0</xdr:col>
                     <xdr:colOff>723900</xdr:colOff>
                     <xdr:row>4</xdr:row>
-                    <xdr:rowOff>9525</xdr:rowOff>
+                    <xdr:rowOff>12700</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
             </control>
           </mc:Choice>
+          <mc:Fallback/>
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1026" r:id="rId5" name="Check Box 2">
+            <control shapeId="1026" r:id="rId4" name="Check Box 2">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>0</xdr:col>
                     <xdr:colOff>419100</xdr:colOff>
                     <xdr:row>3</xdr:row>
-                    <xdr:rowOff>171450</xdr:rowOff>
+                    <xdr:rowOff>177800</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>0</xdr:col>
                     <xdr:colOff>723900</xdr:colOff>
                     <xdr:row>5</xdr:row>
-                    <xdr:rowOff>9525</xdr:rowOff>
+                    <xdr:rowOff>12700</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
             </control>
           </mc:Choice>
+          <mc:Fallback/>
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1027" r:id="rId6" name="Check Box 3">
+            <control shapeId="1027" r:id="rId5" name="Check Box 3">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>0</xdr:col>
                     <xdr:colOff>419100</xdr:colOff>
                     <xdr:row>4</xdr:row>
-                    <xdr:rowOff>171450</xdr:rowOff>
+                    <xdr:rowOff>177800</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>0</xdr:col>
                     <xdr:colOff>723900</xdr:colOff>
                     <xdr:row>6</xdr:row>
-                    <xdr:rowOff>9525</xdr:rowOff>
+                    <xdr:rowOff>12700</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
             </control>
           </mc:Choice>
+          <mc:Fallback/>
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1028" r:id="rId7" name="Check Box 4">
+            <control shapeId="1028" r:id="rId6" name="Check Box 4">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>0</xdr:col>
                     <xdr:colOff>419100</xdr:colOff>
                     <xdr:row>6</xdr:row>
-                    <xdr:rowOff>171450</xdr:rowOff>
+                    <xdr:rowOff>177800</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>0</xdr:col>
                     <xdr:colOff>723900</xdr:colOff>
                     <xdr:row>8</xdr:row>
-                    <xdr:rowOff>9525</xdr:rowOff>
+                    <xdr:rowOff>12700</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
             </control>
           </mc:Choice>
+          <mc:Fallback/>
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1029" r:id="rId8" name="Check Box 5">
+            <control shapeId="1029" r:id="rId7" name="Check Box 5">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>0</xdr:col>
                     <xdr:colOff>419100</xdr:colOff>
                     <xdr:row>7</xdr:row>
-                    <xdr:rowOff>171450</xdr:rowOff>
+                    <xdr:rowOff>177800</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>0</xdr:col>
                     <xdr:colOff>723900</xdr:colOff>
                     <xdr:row>9</xdr:row>
-                    <xdr:rowOff>9525</xdr:rowOff>
+                    <xdr:rowOff>12700</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
             </control>
           </mc:Choice>
+          <mc:Fallback/>
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1030" r:id="rId9" name="Check Box 6">
+            <control shapeId="1030" r:id="rId8" name="Check Box 6">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>0</xdr:col>
                     <xdr:colOff>419100</xdr:colOff>
                     <xdr:row>9</xdr:row>
-                    <xdr:rowOff>171450</xdr:rowOff>
+                    <xdr:rowOff>177800</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>0</xdr:col>
                     <xdr:colOff>723900</xdr:colOff>
                     <xdr:row>11</xdr:row>
-                    <xdr:rowOff>9525</xdr:rowOff>
+                    <xdr:rowOff>12700</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
             </control>
           </mc:Choice>
+          <mc:Fallback/>
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1031" r:id="rId10" name="Check Box 7">
+            <control shapeId="1031" r:id="rId9" name="Check Box 7">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>0</xdr:col>
                     <xdr:colOff>419100</xdr:colOff>
                     <xdr:row>11</xdr:row>
-                    <xdr:rowOff>171450</xdr:rowOff>
+                    <xdr:rowOff>177800</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>0</xdr:col>
                     <xdr:colOff>723900</xdr:colOff>
                     <xdr:row>13</xdr:row>
-                    <xdr:rowOff>9525</xdr:rowOff>
+                    <xdr:rowOff>12700</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
             </control>
           </mc:Choice>
+          <mc:Fallback/>
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1032" r:id="rId11" name="Check Box 8">
+            <control shapeId="1032" r:id="rId10" name="Check Box 8">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>0</xdr:col>
                     <xdr:colOff>419100</xdr:colOff>
                     <xdr:row>13</xdr:row>
-                    <xdr:rowOff>171450</xdr:rowOff>
+                    <xdr:rowOff>177800</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>0</xdr:col>
                     <xdr:colOff>723900</xdr:colOff>
                     <xdr:row>15</xdr:row>
-                    <xdr:rowOff>9525</xdr:rowOff>
+                    <xdr:rowOff>12700</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
             </control>
           </mc:Choice>
+          <mc:Fallback/>
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1033" r:id="rId12" name="Check Box 9">
+            <control shapeId="1033" r:id="rId11" name="Check Box 9">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>0</xdr:col>
                     <xdr:colOff>419100</xdr:colOff>
                     <xdr:row>15</xdr:row>
-                    <xdr:rowOff>171450</xdr:rowOff>
+                    <xdr:rowOff>177800</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>0</xdr:col>
                     <xdr:colOff>723900</xdr:colOff>
                     <xdr:row>17</xdr:row>
-                    <xdr:rowOff>9525</xdr:rowOff>
+                    <xdr:rowOff>12700</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
             </control>
           </mc:Choice>
+          <mc:Fallback/>
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1034" r:id="rId13" name="Check Box 10">
+            <control shapeId="1034" r:id="rId12" name="Check Box 10">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>0</xdr:col>
                     <xdr:colOff>419100</xdr:colOff>
                     <xdr:row>17</xdr:row>
-                    <xdr:rowOff>171450</xdr:rowOff>
+                    <xdr:rowOff>177800</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>0</xdr:col>
                     <xdr:colOff>723900</xdr:colOff>
                     <xdr:row>19</xdr:row>
-                    <xdr:rowOff>9525</xdr:rowOff>
+                    <xdr:rowOff>12700</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
             </control>
           </mc:Choice>
+          <mc:Fallback/>
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1035" r:id="rId14" name="Check Box 11">
+            <control shapeId="1035" r:id="rId13" name="Check Box 11">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>0</xdr:col>
                     <xdr:colOff>419100</xdr:colOff>
                     <xdr:row>20</xdr:row>
-                    <xdr:rowOff>171450</xdr:rowOff>
+                    <xdr:rowOff>177800</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>0</xdr:col>
                     <xdr:colOff>723900</xdr:colOff>
                     <xdr:row>22</xdr:row>
-                    <xdr:rowOff>9525</xdr:rowOff>
+                    <xdr:rowOff>12700</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
             </control>
           </mc:Choice>
+          <mc:Fallback/>
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1036" r:id="rId15" name="Check Box 12">
+            <control shapeId="1036" r:id="rId14" name="Check Box 12">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>0</xdr:col>
                     <xdr:colOff>419100</xdr:colOff>
                     <xdr:row>21</xdr:row>
-                    <xdr:rowOff>171450</xdr:rowOff>
+                    <xdr:rowOff>177800</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>0</xdr:col>
                     <xdr:colOff>723900</xdr:colOff>
                     <xdr:row>23</xdr:row>
-                    <xdr:rowOff>9525</xdr:rowOff>
+                    <xdr:rowOff>12700</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
             </control>
           </mc:Choice>
+          <mc:Fallback/>
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1037" r:id="rId16" name="Check Box 13">
+            <control shapeId="1037" r:id="rId15" name="Check Box 13">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>0</xdr:col>
                     <xdr:colOff>419100</xdr:colOff>
                     <xdr:row>23</xdr:row>
-                    <xdr:rowOff>171450</xdr:rowOff>
+                    <xdr:rowOff>177800</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>0</xdr:col>
                     <xdr:colOff>723900</xdr:colOff>
                     <xdr:row>25</xdr:row>
-                    <xdr:rowOff>9525</xdr:rowOff>
+                    <xdr:rowOff>12700</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
             </control>
           </mc:Choice>
+          <mc:Fallback/>
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1038" r:id="rId17" name="Check Box 14">
+            <control shapeId="1038" r:id="rId16" name="Check Box 14">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>0</xdr:col>
                     <xdr:colOff>419100</xdr:colOff>
                     <xdr:row>24</xdr:row>
-                    <xdr:rowOff>171450</xdr:rowOff>
+                    <xdr:rowOff>177800</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>0</xdr:col>
                     <xdr:colOff>723900</xdr:colOff>
                     <xdr:row>26</xdr:row>
-                    <xdr:rowOff>9525</xdr:rowOff>
+                    <xdr:rowOff>12700</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
             </control>
           </mc:Choice>
+          <mc:Fallback/>
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1039" r:id="rId18" name="Check Box 15">
+            <control shapeId="1039" r:id="rId17" name="Check Box 15">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>0</xdr:col>
                     <xdr:colOff>419100</xdr:colOff>
                     <xdr:row>26</xdr:row>
-                    <xdr:rowOff>171450</xdr:rowOff>
+                    <xdr:rowOff>177800</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>0</xdr:col>
                     <xdr:colOff>723900</xdr:colOff>
                     <xdr:row>28</xdr:row>
-                    <xdr:rowOff>9525</xdr:rowOff>
+                    <xdr:rowOff>12700</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
             </control>
           </mc:Choice>
+          <mc:Fallback/>
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1040" r:id="rId19" name="Check Box 16">
+            <control shapeId="1040" r:id="rId18" name="Check Box 16">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>0</xdr:col>
                     <xdr:colOff>419100</xdr:colOff>
                     <xdr:row>27</xdr:row>
-                    <xdr:rowOff>171450</xdr:rowOff>
+                    <xdr:rowOff>177800</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>0</xdr:col>
                     <xdr:colOff>723900</xdr:colOff>
                     <xdr:row>29</xdr:row>
-                    <xdr:rowOff>9525</xdr:rowOff>
+                    <xdr:rowOff>12700</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
             </control>
           </mc:Choice>
+          <mc:Fallback/>
         </mc:AlternateContent>
       </controls>
     </mc:Choice>
+    <mc:Fallback/>
   </mc:AlternateContent>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -1969,9 +2016,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -1981,8 +2033,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>